<commit_message>
Detalhando Except e adicionando mais personalização a mensagem
</commit_message>
<xml_diff>
--- a/Texto e Lista de contatos.xlsx
+++ b/Texto e Lista de contatos.xlsx
@@ -1,47 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Área de Trabalho\Disparador WhasApp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\espbi\Documents\Disparador_Whatsapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC122447-A41B-44A9-B6C2-1F2027E35672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20490" windowHeight="7650" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Texto" sheetId="1" r:id="rId1"/>
     <sheet name="Lista Contatos" sheetId="2" r:id="rId2"/>
-    <sheet name="Config" sheetId="3" state="hidden" r:id="rId3"/>
+    <sheet name="Config" sheetId="3" r:id="rId3"/>
+    <sheet name="Configurações" sheetId="4" r:id="rId4"/>
+    <sheet name="Rascunho" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <extLst>
-    <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1679534471" val="1062" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1679534471" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1679534471" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1679534471"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Escreva o texto no campo abaixo</t>
   </si>
   <si>
-    <t>Olá --CONTATO--! , tô testando essa mensagem! 
-Isso é um teste de envio pelo whatsApp, com PlanMaker. 浪
-estou apenas verificando os texto em *NEGRITO* e os acentos gramaticais, tipo essa palavra aqui BÊNÇÃO 
-Aproveitando fica com esses emoticons 
-www.google.com
---CONTATO--, muito obrigado por ler tudo! </t>
-  </si>
-  <si>
     <t>Primeiro Nome</t>
   </si>
   <si>
@@ -57,32 +44,96 @@
     <t>5584980808080</t>
   </si>
   <si>
-    <t>Contato 2</t>
+    <t>Teste 2</t>
   </si>
   <si>
     <t>5584994014243</t>
   </si>
   <si>
-    <t>Contato 3</t>
-  </si>
-  <si>
-    <t>Contato 4</t>
-  </si>
-  <si>
-    <t>+5584994014243</t>
+    <t>Teste 3</t>
   </si>
   <si>
     <t>definicoes</t>
   </si>
   <si>
-    <t>Jonas</t>
+    <t>espbi</t>
+  </si>
+  <si>
+    <t>Não</t>
+  </si>
+  <si>
+    <t>Tempo entre mensagens</t>
+  </si>
+  <si>
+    <t>Enviar imagem?</t>
+  </si>
+  <si>
+    <t>segudos</t>
+  </si>
+  <si>
+    <t>Adicional</t>
+  </si>
+  <si>
+    <t>ONIX</t>
+  </si>
+  <si>
+    <t>TRACKER</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Digite </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>--CONTATO--</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> se quiser adicionar o nome do contato no texto ao lado
+Digite </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>--ADD--</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> se quiser inserir o adicional no texto ao lado</t>
+    </r>
+  </si>
+  <si>
+    <t>Olá, --CONTATO--!
+Revisão do --ADD-- por apenas 4x de R$ 49,90 😎
+vem, não perca tempo, vou deixar reservado em nome de --CONTATO-- o horário de 09:15 neste sábado!! 😇</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -96,8 +147,40 @@
       <name val="Century Gothic"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -116,8 +199,14 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -154,49 +243,105 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="16">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
       <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-    <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1679534471" count="1">
-        <pm:charStyle name="Normal" fontId="0" Id="1"/>
-      </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1679534471" count="3">
-        <pm:color name="Cor 24" rgb="44546A"/>
-        <pm:color name="Cor 25" rgb="FFF2CA"/>
-        <pm:color name="Cor 26" rgb="A5A5A5"/>
-      </pm:colors>
     </ext>
   </extLst>
 </styleSheet>
@@ -457,120 +602,115 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFC2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:XFD3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="93.140625" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="16383" width="9.140625" hidden="1"/>
+    <col min="16384" max="16384" width="0.140625" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="395.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <sheetProtection sheet="1" formatCells="0" autoFilter="0"/>
+  <pageMargins left="0.51180599999999998" right="0.51180599999999998" top="0.78749999999999998" bottom="0.78749999999999998" header="0.315278" footer="0.315278"/>
+  <pageSetup paperSize="9" fitToWidth="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="93.140625" customWidth="1"/>
-    <col min="2" max="16383" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="16384" max="16384" width="0.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="8" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="395.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1"/>
+      <c r="E1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" autoFilter="0"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.51180599999999998" right="0.51180599999999998" top="0.78749999999999998" bottom="0.78749999999999998" header="0.315278" footer="0.315278"/>
-  <pageSetup paperSize="9" fitToWidth="0"/>
-  <extLst>
-    <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1679534471" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
-        <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
-        <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
-      </pm:sheetPrefs>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" style="3" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.51180599999999998" right="0.51180599999999998" top="0.78749999999999998" bottom="0.78749999999999998" header="0.315278" footer="0.315278"/>
-  <pageSetup paperSize="9" fitToWidth="0"/>
-  <extLst>
-    <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1679534471" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
-        <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
-        <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
-      </pm:sheetPrefs>
-    </ext>
-  </extLst>
+  <pageSetup paperSize="9" fitToWidth="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -584,24 +724,79 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.51180599999999998" right="0.51180599999999998" top="0.78749999999999998" bottom="0.78749999999999998" header="0.315278" footer="0.315278"/>
   <pageSetup paperSize="9" fitToWidth="0"/>
-  <extLst>
-    <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1679534471" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
-        <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
-        <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
-      </pm:sheetPrefs>
-    </ext>
-  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{197D0BF9-F460-4D0D-888F-058F3CD1C58A}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.85546875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="13">
+        <v>5</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1" xr:uid="{4337EDC8-E801-429D-ABCE-87CE0B059CB0}">
+      <formula1>"Sim,Não"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Tempo fora do ideal" error="O minimo aceitável é de 5 segundos" sqref="C2" xr:uid="{B1BC4E5C-C024-426E-8CAD-24ADD0E4D689}">
+      <formula1>5</formula1>
+      <formula2>1000</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64B914EA-4F83-4544-90D7-782BA8A0FAEE}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Renomeei 'app' para 'Iniciar' e adicionei uma função 'Proxy'
</commit_message>
<xml_diff>
--- a/Texto e Lista de contatos.xlsx
+++ b/Texto e Lista de contatos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\espbi\Documents\Disparador_Whatsapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC122447-A41B-44A9-B6C2-1F2027E35672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4214DA-9E1C-4555-A46E-72B1BC372128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Texto" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Escreva o texto no campo abaixo</t>
   </si>
@@ -38,30 +38,18 @@
     <t>+5584988083657</t>
   </si>
   <si>
-    <t>NumErrado</t>
-  </si>
-  <si>
-    <t>5584980808080</t>
-  </si>
-  <si>
     <t>Teste 2</t>
   </si>
   <si>
     <t>5584994014243</t>
   </si>
   <si>
-    <t>Teste 3</t>
-  </si>
-  <si>
     <t>definicoes</t>
   </si>
   <si>
     <t>espbi</t>
   </si>
   <si>
-    <t>Não</t>
-  </si>
-  <si>
     <t>Tempo entre mensagens</t>
   </si>
   <si>
@@ -75,9 +63,6 @@
   </si>
   <si>
     <t>ONIX</t>
-  </si>
-  <si>
-    <t>TRACKER</t>
   </si>
   <si>
     <r>
@@ -127,6 +112,9 @@
     <t>Olá, --CONTATO--!
 Revisão do --ADD-- por apenas 4x de R$ 49,90 😎
 vem, não perca tempo, vou deixar reservado em nome de --CONTATO-- o horário de 09:15 neste sábado!! 😇</t>
+  </si>
+  <si>
+    <t>Não</t>
   </si>
 </sst>
 </file>
@@ -305,7 +293,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -603,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:XFD3"/>
+  <dimension ref="A1:XFC3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -624,10 +612,10 @@
     </row>
     <row r="2" spans="1:2" ht="395.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25"/>
@@ -640,10 +628,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,7 +650,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D1"/>
       <c r="E1"/>
@@ -672,34 +660,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -724,12 +693,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -742,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{197D0BF9-F460-4D0D-888F-058F3CD1C58A}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -757,21 +726,21 @@
   <sheetData>
     <row r="1" spans="2:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="2:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C2" s="13">
         <v>5</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>